<commit_message>
added task02 code; added some r summary code
</commit_message>
<xml_diff>
--- a/Task_02/data/Merged GDP and Birth Rate.xlsx
+++ b/Task_02/data/Merged GDP and Birth Rate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\Studium\Data Analysis\Task02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Studium\DataAnalysis\Task_02\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="458">
   <si>
-    <t>Country Name</t>
-  </si>
-  <si>
-    <t>Country Code</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
@@ -1394,10 +1388,16 @@
     <t>ZWE</t>
   </si>
   <si>
-    <t>GDP per Capita</t>
-  </si>
-  <si>
-    <t>Birth Rate</t>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>gdp_per_capita</t>
+  </si>
+  <si>
+    <t>birth_rate</t>
   </si>
 </sst>
 </file>
@@ -1470,10 +1470,10 @@
     <sortCondition ref="A1:A228"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Country Name" dataCellStyle="Standard 2"/>
-    <tableColumn id="2" name="Country Code" dataCellStyle="Standard 2"/>
-    <tableColumn id="3" name="GDP per Capita" dataCellStyle="Standard 2"/>
-    <tableColumn id="4" name="Birth Rate" dataCellStyle="Standard 2"/>
+    <tableColumn id="1" name="country_name" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" name="country_code" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" name="gdp_per_capita" dataCellStyle="Standard 2"/>
+    <tableColumn id="4" name="birth_rate" dataCellStyle="Standard 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1745,7 +1745,7 @@
   <dimension ref="A1:D228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,10 +1758,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>454</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>455</v>
       </c>
       <c r="C1" t="s">
         <v>456</v>
@@ -1772,10 +1772,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3">
         <v>633.94786429463898</v>
@@ -1786,10 +1786,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>4588.6494401481114</v>
@@ -1800,10 +1800,10 @@
     </row>
     <row r="4" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3">
         <v>5484.0668056148024</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>5232.6905005413246</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>13432.079207920791</v>
@@ -1842,10 +1842,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>7478.9975166389731</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>12324.938785772762</v>
@@ -1870,10 +1870,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="3">
         <v>3873.5335658068184</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3">
         <v>61995.829697600006</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3">
         <v>51148.358876079612</v>
@@ -1912,10 +1912,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3">
         <v>7886.4591436727369</v>
@@ -1926,10 +1926,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3">
         <v>22217.494139207527</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3">
         <v>24855.215635008579</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>1086.8000867693543</v>
@@ -1968,10 +1968,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3">
         <v>15366.292610628838</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3">
         <v>8025.3043555246841</v>
@@ -1996,10 +1996,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="3">
         <v>47299.860108561152</v>
@@ -2010,10 +2010,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3">
         <v>4884.368620381797</v>
@@ -2024,10 +2024,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="3">
         <v>903.46492400769262</v>
@@ -2038,10 +2038,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3">
         <v>2560.5221317413138</v>
@@ -2052,10 +2052,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3">
         <v>3124.0807621235276</v>
@@ -2066,10 +2066,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3">
         <v>4851.660527869255</v>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3">
         <v>7153.4443253521167</v>
@@ -2094,10 +2094,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3">
         <v>11728.799387510755</v>
@@ -2108,10 +2108,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3">
         <v>40979.64194333784</v>
@@ -2122,10 +2122,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3">
         <v>7851.265428042344</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="3">
         <v>713.45644162667475</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" s="3">
         <v>286.00233587295247</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="3">
         <v>3641.1076558657514</v>
@@ -2178,10 +2178,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C31" s="3">
         <v>1094.576687778989</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3">
         <v>1407.4034132223412</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" s="3">
         <v>50185.481497034634</v>
@@ -2220,10 +2220,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3">
         <v>10171.005042635563</v>
@@ -2234,10 +2234,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="3">
         <v>351.99422601786637</v>
@@ -2248,10 +2248,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3">
         <v>14084.05848802089</v>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C37" s="3">
         <v>1024.668354021906</v>
@@ -2276,10 +2276,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" s="3">
         <v>14566.149054918318</v>
@@ -2290,10 +2290,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39" s="3">
         <v>7587.2897316633535</v>
@@ -2304,10 +2304,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="3">
         <v>7918.0789003935233</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="3">
         <v>810.07576003061206</v>
@@ -2332,10 +2332,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C42" s="3">
         <v>437.81493117827245</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C43" s="3">
         <v>3147.0715240876407</v>
@@ -2360,10 +2360,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="3">
         <v>10415.456649677291</v>
@@ -2374,10 +2374,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" s="3">
         <v>1545.9422492516239</v>
@@ -2388,10 +2388,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C46" s="3">
         <v>13480.650753628146</v>
@@ -2402,10 +2402,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C47" s="3">
         <v>27245.744624900901</v>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" s="3">
         <v>19502.417330608314</v>
@@ -2430,10 +2430,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C49" s="3">
         <v>61330.912625204408</v>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C50" s="3">
         <v>1813.596226144276</v>
@@ -2458,10 +2458,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C51" s="3">
         <v>6147.3435691578989</v>
@@ -2472,10 +2472,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C52" s="3">
         <v>3329.3001789603463</v>
@@ -2486,10 +2486,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" s="3">
         <v>9491.6693449381019</v>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" s="3">
         <v>6242.2713217776427</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C55" s="3">
         <v>6308.6610655870099</v>
@@ -2528,10 +2528,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C56" s="3">
         <v>6345.8407250594801</v>
@@ -2542,10 +2542,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="3">
         <v>3365.7074205747667</v>
@@ -2556,10 +2556,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C58" s="3">
         <v>4102.0638517964026</v>
@@ -2570,10 +2570,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C59" s="3">
         <v>18918.276831332783</v>
@@ -2584,10 +2584,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="3">
         <v>20147.77821675529</v>
@@ -2598,10 +2598,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C61" s="3">
         <v>573.56596034607651</v>
@@ -2612,10 +2612,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" s="3">
         <v>39594.645843478924</v>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C63" s="3">
         <v>25846.097188443851</v>
@@ -2640,10 +2640,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" s="3">
         <v>9426.0775534913628</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C65" s="3">
         <v>9877.8724499605451</v>
@@ -2668,10 +2668,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C66" s="3">
         <v>36425.565954593985</v>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C67" s="3">
         <v>5112.3818903725105</v>
@@ -2696,10 +2696,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C68" s="3">
         <v>49864.576245357937</v>
@@ -2710,10 +2710,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C69" s="3">
         <v>1643.5280080944176</v>
@@ -2724,10 +2724,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C70" s="3">
         <v>42546.8387870273</v>
@@ -2738,10 +2738,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C71" s="3">
         <v>10772.061753763734</v>
@@ -2752,10 +2752,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C72" s="3">
         <v>441.29381701438189</v>
@@ -2766,10 +2766,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C73" s="3">
         <v>4429.6500745149051</v>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C74" s="3">
         <v>47767.001905643498</v>
@@ -2794,10 +2794,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C75" s="3">
         <v>1441.6364531116637</v>
@@ -2808,10 +2808,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C76" s="3">
         <v>21627.354287641716</v>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C77" s="3">
         <v>43364.882849917551</v>
@@ -2836,10 +2836,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C78" s="3">
         <v>8573.6939489584074</v>
@@ -2850,10 +2850,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C79" s="3">
         <v>3666.5946063331185</v>
@@ -2864,10 +2864,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C80" s="3">
         <v>539.61577498875556</v>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C81" s="3">
         <v>615.94092219971719</v>
@@ -2892,10 +2892,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C82" s="3">
         <v>4028.1639914829043</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C83" s="3">
         <v>830.15005511436766</v>
@@ -2920,10 +2920,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C84" s="3">
         <v>900.09085284188905</v>
@@ -2934,10 +2934,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C85" s="3">
         <v>42329.590877631745</v>
@@ -2948,10 +2948,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C86" s="3">
         <v>2434.2800463030003</v>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C87" s="3">
         <v>40215.667731126494</v>
@@ -2976,10 +2976,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C88" s="3">
         <v>14021.902274346996</v>
@@ -2990,10 +2990,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C89" s="3">
         <v>5937.393949032763</v>
@@ -3004,10 +3004,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C90" s="3">
         <v>52036.731814453124</v>
@@ -3018,10 +3018,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C91" s="3">
         <v>4747.0704869956007</v>
@@ -3032,10 +3032,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C92" s="3">
         <v>2227.5956010628629</v>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C93" s="3">
         <v>946.96284707687448</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C94" s="3">
         <v>1411.6990643130046</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C95" s="3">
         <v>1576.8176688728552</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C96" s="3">
         <v>3499.5887347651465</v>
@@ -3102,10 +3102,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C97" s="3">
         <v>5442.8747707603861</v>
@@ -3116,10 +3116,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C98" s="3">
         <v>6336.4680661563352</v>
@@ -3130,10 +3130,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C99" s="3">
         <v>54321.287718512416</v>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C100" s="3">
         <v>37206.182941806859</v>
@@ -3158,10 +3158,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C101" s="3">
         <v>35179.653951530156</v>
@@ -3172,10 +3172,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C102" s="3">
         <v>5119.2184171201998</v>
@@ -3186,10 +3186,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C103" s="3">
         <v>36152.690017146779</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C104" s="3">
         <v>4830.9769152594299</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C105" s="3">
         <v>13154.844592288686</v>
@@ -3228,10 +3228,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C106" s="3">
         <v>1368.4911321579687</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C107" s="3">
         <v>1509.5211865704705</v>
@@ -3256,10 +3256,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C108" s="3">
         <v>27989.353992586286</v>
@@ -3270,10 +3270,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C109" s="3">
         <v>4073.8191168688304</v>
@@ -3284,10 +3284,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C110" s="3">
         <v>43593.702017651369</v>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C111" s="3">
         <v>1279.7697826598551</v>
@@ -3312,10 +3312,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C112" s="3">
         <v>1751.3969706633591</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C113" s="3">
         <v>8720.0387318845715</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C114" s="3">
         <v>9953.678065377977</v>
@@ -3354,10 +3354,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C115" s="3">
         <v>9605.1798948384112</v>
@@ -3368,10 +3368,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C116" s="3">
         <v>9867.9669686754369</v>
@@ -3382,10 +3382,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C117" s="3">
         <v>15692.191561178135</v>
@@ -3396,10 +3396,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C118" s="3">
         <v>992.20291310814366</v>
@@ -3410,10 +3410,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C119" s="3">
         <v>8148.6391668338956</v>
@@ -3424,10 +3424,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C120" s="3">
         <v>1034.1852875122145</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C121" s="3">
         <v>457.8585865202611</v>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C122" s="3">
         <v>6573.386737262007</v>
@@ -3466,10 +3466,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C123" s="3">
         <v>16489.728983533121</v>
@@ -3480,10 +3480,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C124" s="3">
         <v>4628.482658128105</v>
@@ -3494,10 +3494,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C125" s="3">
         <v>654.31311118946735</v>
@@ -3508,10 +3508,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C126" s="3">
         <v>2032.5139154735409</v>
@@ -3522,10 +3522,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C127" s="3">
         <v>116612.88415187472</v>
@@ -3536,10 +3536,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C128" s="3">
         <v>96074.836959719556</v>
@@ -3550,10 +3550,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C129" s="3">
         <v>5453.2812751277434</v>
@@ -3564,10 +3564,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C130" s="3">
         <v>467.13033427081643</v>
@@ -3578,10 +3578,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C131" s="3">
         <v>362.24748659502455</v>
@@ -3592,10 +3592,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C132" s="3">
         <v>11307.064952827986</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C133" s="3">
         <v>7640.6471532800988</v>
@@ -3620,10 +3620,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C134" s="3">
         <v>842.11433723773666</v>
@@ -3634,10 +3634,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C135" s="3">
         <v>1370.9852124851118</v>
@@ -3648,10 +3648,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C136" s="3">
         <v>10002.870475047099</v>
@@ -3662,10 +3662,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C137" s="3">
         <v>10350.814693017952</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C138" s="3">
         <v>3057.091024717879</v>
@@ -3690,10 +3690,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C139" s="3">
         <v>8470.1600590162925</v>
@@ -3704,10 +3704,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C140" s="3">
         <v>4378.61083035712</v>
@@ -3718,10 +3718,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C141" s="3">
         <v>4395.550768765871</v>
@@ -3732,10 +3732,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C142" s="3">
         <v>5080.7848149669162</v>
@@ -3746,10 +3746,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C143" s="3">
         <v>2244.7637624833401</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C144" s="3">
         <v>4201.7377108932687</v>
@@ -3774,10 +3774,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C145" s="3">
         <v>7378.0444044103406</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C146" s="3">
         <v>3190.3104441402402</v>
@@ -3802,10 +3802,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C147" s="3">
         <v>622.63806443774638</v>
@@ -3816,10 +3816,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C148" s="3">
         <v>1203.8447211036409</v>
@@ -3830,10 +3830,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C149" s="3">
         <v>5342.9444603987158</v>
@@ -3844,10 +3844,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C150" s="3">
         <v>701.68006339949591</v>
@@ -3858,10 +3858,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C151" s="3">
         <v>52138.683924409554</v>
@@ -3872,10 +3872,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C152" s="3">
         <v>44380.426584211964</v>
@@ -3886,10 +3886,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C153" s="3">
         <v>1960.490907713126</v>
@@ -3900,10 +3900,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C154" s="3">
         <v>431.38168213785582</v>
@@ -3914,10 +3914,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C155" s="3">
         <v>3203.2442957326134</v>
@@ -3928,10 +3928,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C156" s="3">
         <v>53982.331652978311</v>
@@ -3942,10 +3942,10 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C157" s="3">
         <v>97429.708475945372</v>
@@ -3956,10 +3956,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C158" s="3">
         <v>38271.804726328803</v>
@@ -3970,10 +3970,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C159" s="3">
         <v>19309.612449902281</v>
@@ -3984,10 +3984,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C160" s="3">
         <v>15653.198290070857</v>
@@ -3998,10 +3998,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C161" s="3">
         <v>3807.0473133144528</v>
@@ -4012,10 +4012,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C162" s="3">
         <v>1315.2676219428365</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C163" s="3">
         <v>12712.431328998962</v>
@@ -4040,10 +4040,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C164" s="3">
         <v>2268.1725394430214</v>
@@ -4054,10 +4054,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C165" s="3">
         <v>4712.8702053640463</v>
@@ -4068,10 +4068,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C166" s="3">
         <v>6549.3892292809032</v>
@@ -4082,10 +4082,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C167" s="3">
         <v>2872.5121647165715</v>
@@ -4096,10 +4096,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C168" s="3">
         <v>14337.20636743083</v>
@@ -4110,10 +4110,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C169" s="3">
         <v>22124.367092545061</v>
@@ -4124,10 +4124,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C170" s="3">
         <v>42362.433997626431</v>
@@ -4138,10 +4138,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C171" s="3">
         <v>1771.5223038875076</v>
@@ -4152,10 +4152,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C172" s="3">
         <v>96732.529026221891</v>
@@ -4166,10 +4166,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C173" s="3">
         <v>10011.785922629884</v>
@@ -4180,10 +4180,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C174" s="3">
         <v>13902.1428503026</v>
@@ -4194,10 +4194,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C175" s="3">
         <v>697.62650127370637</v>
@@ -4208,10 +4208,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C176" s="3">
         <v>4172.2171003766134</v>
@@ -4222,10 +4222,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C177" s="3">
         <v>1810.7215616492078</v>
@@ -4236,10 +4236,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C178" s="3">
         <v>24406.467821721937</v>
@@ -4250,10 +4250,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C179" s="3">
         <v>1067.1317533269985</v>
@@ -4264,10 +4264,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C180" s="3">
         <v>6200.1732210247383</v>
@@ -4278,10 +4278,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C181" s="3">
         <v>15563.794218367593</v>
@@ -4292,10 +4292,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C182" s="3">
         <v>792.58355040933395</v>
@@ -4306,10 +4306,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C183" s="3">
         <v>56007.288209026963</v>
@@ -4320,10 +4320,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C184" s="3">
         <v>18501.429615533638</v>
@@ -4334,10 +4334,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C185" s="3">
         <v>24001.880133687959</v>
@@ -4348,10 +4348,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C186" s="3">
         <v>13891.15082958635</v>
@@ -4362,10 +4362,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C187" s="3">
         <v>2024.2028612336212</v>
@@ -4376,10 +4376,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C188" s="3">
         <v>542.61588395569356</v>
@@ -4390,10 +4390,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C189" s="3">
         <v>6472.1010273462352</v>
@@ -4404,10 +4404,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C190" s="3">
         <v>1501.0740895376923</v>
@@ -4418,10 +4418,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C191" s="3">
         <v>1501.0740895376923</v>
@@ -4432,10 +4432,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C192" s="3">
         <v>1115.0935149602515</v>
@@ -4446,10 +4446,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C193" s="3">
         <v>29718.500215544143</v>
@@ -4460,10 +4460,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C194" s="3">
         <v>3852.8807604116218</v>
@@ -4474,10 +4474,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C195" s="3">
         <v>7647.5295028754153</v>
@@ -4488,10 +4488,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C196" s="3">
         <v>6672.8105374028009</v>
@@ -4502,10 +4502,10 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C197" s="3">
         <v>1800.6330379110143</v>
@@ -4516,10 +4516,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C198" s="3">
         <v>1799.3413641817133</v>
@@ -4530,10 +4530,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C199" s="3">
         <v>1800.6330379110143</v>
@@ -4544,10 +4544,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C200" s="3">
         <v>1875.84328741646</v>
@@ -4558,10 +4558,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C201" s="3">
         <v>9680.1159136736806</v>
@@ -4572,10 +4572,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C202" s="3">
         <v>3477.1492455895573</v>
@@ -4586,10 +4586,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C203" s="3">
         <v>58899.979794484476</v>
@@ -4600,10 +4600,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C204" s="3">
         <v>85610.842028526138</v>
@@ -4614,10 +4614,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C205" s="3">
         <v>1113.3663544671515</v>
@@ -4628,10 +4628,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C206" s="3">
         <v>954.61898795461605</v>
@@ -4642,10 +4642,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C207" s="3">
         <v>5969.9401158379096</v>
@@ -4656,10 +4656,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C208" s="3">
         <v>1131.230850718237</v>
@@ -4670,10 +4670,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C209" s="3">
         <v>629.99764394670012</v>
@@ -4684,10 +4684,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C210" s="3">
         <v>4114.0521151127878</v>
@@ -4698,10 +4698,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C211" s="3">
         <v>21317.449265567964</v>
@@ -4712,10 +4712,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C212" s="3">
         <v>4328.904197348812</v>
@@ -4726,10 +4726,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C213" s="3">
         <v>10303.898800250052</v>
@@ -4740,10 +4740,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C214" s="3">
         <v>8193.7202969044483</v>
@@ -4754,10 +4754,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C215" s="3">
         <v>714.56735647115602</v>
@@ -4768,10 +4768,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C216" s="3">
         <v>3065.1642226526601</v>
@@ -4782,10 +4782,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C217" s="3">
         <v>43962.713693201076</v>
@@ -4796,10 +4796,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C218" s="3">
         <v>46278.520212882868</v>
@@ -4810,10 +4810,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C219" s="3">
         <v>54398.460009399409</v>
@@ -4824,10 +4824,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C220" s="3">
         <v>8494.6540189726293</v>
@@ -4838,10 +4838,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C221" s="3">
         <v>16737.973101175034</v>
@@ -4852,10 +4852,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C222" s="3">
         <v>2052.5867813592472</v>
@@ -4866,10 +4866,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C223" s="3">
         <v>3147.9648598683561</v>
@@ -4880,10 +4880,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C224" s="3">
         <v>2052.3190838008854</v>
@@ -4894,10 +4894,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C225" s="3">
         <v>2960.7780040524535</v>
@@ -4908,10 +4908,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C226" s="3">
         <v>10754.838043409725</v>
@@ -4922,10 +4922,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C227" s="3">
         <v>1725.9745486400898</v>
@@ -4936,10 +4936,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C228" s="3">
         <v>931.19818468691994</v>

</xml_diff>